<commit_message>
update bond trade record
</commit_message>
<xml_diff>
--- a/report/bond/bond.xlsx
+++ b/report/bond/bond.xlsx
@@ -366,10 +366,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L43"/>
+  <dimension ref="A1:L44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -420,17 +420,17 @@
         <v>1713.1699999999837</v>
       </c>
       <c r="F2" s="2">
-        <f>SUM(F22:F23)</f>
-        <v>200.46000000000276</v>
+        <f>SUM(F22:F24)</f>
+        <v>480.86000000000058</v>
       </c>
       <c r="G2" s="2">
-        <f>SUM(G4:G23)</f>
-        <v>34430.429999999978</v>
+        <f>SUM(G4:G24)</f>
+        <v>34710.829999999973</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B3" s="3">
-        <f>XIRR(B4:B24,A4:A24)</f>
+        <f>XIRR(B4:B25,A4:A25)</f>
         <v>0.58600277304649373</v>
       </c>
       <c r="C3" s="3">
@@ -446,12 +446,12 @@
         <v>0.12853825688362122</v>
       </c>
       <c r="F3" s="3">
-        <f>XIRR(F22:F23,A22:A23)</f>
-        <v>0.71156989336013821</v>
+        <f>XIRR(F22:F24,A22:A24)</f>
+        <v>0.23071449398994448</v>
       </c>
       <c r="G3" s="3">
-        <f>XIRR(G4:G23,A4:A23)</f>
-        <v>0.18828975558280944</v>
+        <f>XIRR(G4:G24,A4:A24)</f>
+        <v>0.18803424239158631</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -783,28 +783,37 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
-        <f>DATE(2014,7,31)</f>
-        <v>41851</v>
+        <f>DATE(2014,8,1)</f>
+        <v>41852</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2">
-        <v>19550.240000000002</v>
+        <v>-49397.11</v>
       </c>
       <c r="G23" s="2">
         <f>SUM(F23)</f>
-        <v>19550.240000000002</v>
+        <v>-49397.11</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="5">
+        <f>DATE(2014,8,11)</f>
+        <v>41862</v>
+      </c>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
+      <c r="F24" s="2">
+        <v>69227.75</v>
+      </c>
+      <c r="G24" s="2">
+        <f>SUM(F24)</f>
+        <v>69227.75</v>
+      </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B25" s="2"/>
@@ -957,6 +966,14 @@
       <c r="E43" s="2"/>
       <c r="F43" s="2"/>
       <c r="G43" s="2"/>
+    </row>
+    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2"/>
+      <c r="G44" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>